<commit_message>
feat: update template (import partner)
</commit_message>
<xml_diff>
--- a/public/assets/template/excel/sample.xlsx
+++ b/public/assets/template/excel/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My PC\Documents\ITTP\skripsi\cazh_crm\public\assets\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74224C-4045-455F-A048-7E97E1B66126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AFE77F-04A2-4A1E-BEBF-DBEFB351E8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02C6D976-823C-42EC-9A77-A7CAE796E8F6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Tanggal Onboarding</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>After Sales</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>Imam</t>
+  </si>
+  <si>
+    <t>Dita</t>
   </si>
 </sst>
 </file>
@@ -164,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -202,6 +217,13 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABBBD2-F3B7-4CEE-AB28-64477D4F7101}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,7 +558,7 @@
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33.75">
+    <row r="1" spans="1:14" ht="33.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,8 +595,14 @@
       <c r="L1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="M1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" s="6">
         <v>43848</v>
       </c>
@@ -611,8 +639,14 @@
       <c r="L2" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="M2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="6">
         <v>44064</v>
       </c>
@@ -626,10 +660,7 @@
       <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="str">
-        <f>E2</f>
-        <v>99.999.999.9-999.999</v>
-      </c>
+      <c r="E3" s="7"/>
       <c r="F3" s="7" t="str">
         <f>F2</f>
         <v>password</v>
@@ -652,6 +683,38 @@
       <c r="L3" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="M3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
fix: set nullable field password (import partner)
</commit_message>
<xml_diff>
--- a/public/assets/template/excel/sample.xlsx
+++ b/public/assets/template/excel/sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My PC\Documents\ITTP\skripsi\cazh_crm\public\assets\template\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AFE77F-04A2-4A1E-BEBF-DBEFB351E8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624DB9EF-BBBF-481F-8925-4EA808A0FB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{02C6D976-823C-42EC-9A77-A7CAE796E8F6}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="15375" windowHeight="7875" xr2:uid="{02C6D976-823C-42EC-9A77-A7CAE796E8F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCABBBD2-F3B7-4CEE-AB28-64477D4F7101}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="106" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,10 +661,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="7" t="str">
-        <f>F2</f>
-        <v>password</v>
-      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="7">
         <v>85182951124</v>
       </c>
@@ -723,21 +720,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050935D35F384AF4BBC451617A5CE5789" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="36129ec10bbeef0e9ea748d7e210619b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="21072794-4655-4b81-b930-2614394ba3c3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="74da23e7bf6ab3e31fda5cf45c033a6a" ns3:_="">
     <xsd:import namespace="21072794-4655-4b81-b930-2614394ba3c3"/>
@@ -875,31 +857,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3A76C18-4B3C-42B6-8028-D29B20A02B6D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="21072794-4655-4b81-b930-2614394ba3c3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFED54D6-58BC-423A-A79D-6A043179B50C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC1EB740-B332-40DB-8E7F-DF8A1F0FDAE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -915,4 +888,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFED54D6-58BC-423A-A79D-6A043179B50C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3A76C18-4B3C-42B6-8028-D29B20A02B6D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="21072794-4655-4b81-b930-2614394ba3c3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>